<commit_message>
student BOM minor edits
</commit_message>
<xml_diff>
--- a/eps-eda/bom/eps_BOM.xlsx
+++ b/eps-eda/bom/eps_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igeorgi1\git-repos\coloradocube\eps\eps-eda\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C097C419-7B11-45EA-B790-EBF19AEEA8A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57843CE-4C37-4F63-ACAD-FB31D7F29499}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17445" yWindow="585" windowWidth="24930" windowHeight="14580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17040" yWindow="180" windowWidth="24045" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eps_masterBOM" sheetId="2" r:id="rId1"/>
@@ -533,7 +533,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -571,6 +571,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -611,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -628,25 +635,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,8 +875,9 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:G48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -887,11 +896,11 @@
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -900,10 +909,10 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -913,10 +922,10 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -926,12 +935,12 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -956,288 +965,288 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="23" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
+      <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>6</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="15"/>
+      <c r="G7" s="19"/>
       <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="12" t="s">
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="15"/>
+      <c r="G8" s="19"/>
       <c r="H8" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="11">
         <v>3</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="19"/>
       <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="15"/>
+      <c r="G10" s="19"/>
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="11">
         <v>2</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="19"/>
       <c r="H11" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="13">
+      <c r="B12" s="11">
         <v>4</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="19"/>
       <c r="H12" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="12" t="s">
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="E13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="15"/>
+      <c r="G13" s="19"/>
       <c r="H13" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" s="12" t="s">
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="E14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="19"/>
       <c r="H14" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+      <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="13">
-        <v>1</v>
-      </c>
-      <c r="C15" s="12" t="s">
+      <c r="B15" s="11">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="14" t="s">
+      <c r="F15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="19"/>
       <c r="H15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>3</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="15"/>
+      <c r="G16" s="19"/>
       <c r="H16" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>3</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="15"/>
+      <c r="G17" s="19"/>
       <c r="H17" s="8" t="s">
         <v>26</v>
       </c>
@@ -1258,10 +1267,10 @@
       <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="11"/>
+      <c r="G18" s="17"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1302,10 +1311,10 @@
       <c r="E20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="11"/>
+      <c r="G20" s="17"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1324,10 +1333,10 @@
       <c r="E21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="11"/>
+      <c r="G21" s="17"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1346,10 +1355,10 @@
       <c r="E22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="11"/>
+      <c r="G22" s="17"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1390,10 +1399,10 @@
       <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="11"/>
+      <c r="G24" s="17"/>
       <c r="H24" s="4" t="s">
         <v>71</v>
       </c>
@@ -1414,10 +1423,10 @@
       <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="11"/>
+      <c r="G25" s="17"/>
       <c r="H25" s="8" t="s">
         <v>55</v>
       </c>
@@ -1460,10 +1469,10 @@
       <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="11"/>
+      <c r="G27" s="17"/>
       <c r="H27" s="8" t="s">
         <v>55</v>
       </c>
@@ -1484,10 +1493,10 @@
       <c r="E28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="11"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="8" t="s">
         <v>55</v>
       </c>
@@ -1508,10 +1517,10 @@
       <c r="E29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="11"/>
+      <c r="G29" s="17"/>
       <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
@@ -1532,10 +1541,10 @@
       <c r="E30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="11"/>
+      <c r="G30" s="17"/>
       <c r="H30" s="8" t="s">
         <v>55</v>
       </c>
@@ -1578,392 +1587,392 @@
       <c r="E32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="17"/>
       <c r="H32" s="8" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="17">
+      <c r="B33" s="13">
         <v>2</v>
       </c>
-      <c r="C33" s="16" t="s">
+      <c r="C33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D33" s="16" t="s">
+      <c r="D33" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
       <c r="H33" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="B34" s="17">
+      <c r="B34" s="13">
         <v>5</v>
       </c>
-      <c r="C34" s="16" t="s">
+      <c r="C34" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E34" s="16" t="s">
+      <c r="E34" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="18" t="s">
+      <c r="F34" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="19"/>
+      <c r="G34" s="21"/>
       <c r="H34" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="17">
+      <c r="B35" s="13">
         <v>2</v>
       </c>
-      <c r="C35" s="16" t="s">
+      <c r="C35" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="16" t="s">
+      <c r="D35" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E35" s="16" t="s">
+      <c r="E35" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="18" t="s">
+      <c r="F35" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="19"/>
+      <c r="G35" s="21"/>
       <c r="H35" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B36" s="17">
-        <v>1</v>
-      </c>
-      <c r="C36" s="16" t="s">
+      <c r="B36" s="13">
+        <v>1</v>
+      </c>
+      <c r="C36" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="D36" s="16" t="s">
+      <c r="D36" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E36" s="16" t="s">
+      <c r="E36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="18" t="s">
+      <c r="F36" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="19"/>
+      <c r="G36" s="21"/>
       <c r="H36" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="16" t="s">
+      <c r="A37" s="12" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="17">
-        <v>1</v>
-      </c>
-      <c r="C37" s="16" t="s">
+      <c r="B37" s="13">
+        <v>1</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E37" s="16" t="s">
+      <c r="E37" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="18" t="s">
+      <c r="F37" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="19"/>
+      <c r="G37" s="21"/>
       <c r="H37" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
+      <c r="A38" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="21">
-        <v>1</v>
-      </c>
-      <c r="C38" s="21">
+      <c r="B38" s="15">
+        <v>1</v>
+      </c>
+      <c r="C38" s="15">
         <v>0.01</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="14" t="s">
         <v>120</v>
       </c>
       <c r="F38" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="19"/>
+      <c r="G38" s="21"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
+      <c r="A39" s="12" t="s">
         <v>121</v>
       </c>
-      <c r="B39" s="17">
+      <c r="B39" s="13">
         <v>2</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="13">
         <v>60</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E39" s="16" t="s">
+      <c r="E39" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G39" s="16"/>
+      <c r="G39" s="12"/>
       <c r="H39" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
+      <c r="A40" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="B40" s="17">
-        <v>1</v>
-      </c>
-      <c r="C40" s="16" t="s">
+      <c r="B40" s="13">
+        <v>1</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E40" s="16" t="s">
+      <c r="E40" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G40" s="16"/>
+      <c r="G40" s="12"/>
       <c r="H40" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
+      <c r="A41" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="B41" s="17">
-        <v>1</v>
-      </c>
-      <c r="C41" s="17">
+      <c r="B41" s="13">
+        <v>1</v>
+      </c>
+      <c r="C41" s="13">
         <v>200</v>
       </c>
-      <c r="D41" s="16" t="s">
+      <c r="D41" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="16" t="s">
+      <c r="E41" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G41" s="16"/>
+      <c r="G41" s="12"/>
       <c r="H41" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="16" t="s">
+      <c r="A42" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="17">
+      <c r="B42" s="13">
         <v>5</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="13">
         <v>330</v>
       </c>
-      <c r="D42" s="16" t="s">
+      <c r="D42" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="E42" s="16" t="s">
+      <c r="E42" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="G42" s="16"/>
+      <c r="G42" s="12"/>
       <c r="H42" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="B43" s="17">
-        <v>1</v>
-      </c>
-      <c r="C43" s="16" t="s">
+      <c r="B43" s="13">
+        <v>1</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="D43" s="16" t="s">
+      <c r="D43" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E43" s="16" t="s">
+      <c r="E43" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="18" t="s">
+      <c r="F43" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="19"/>
+      <c r="G43" s="21"/>
       <c r="H43" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I43" s="1"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="B44" s="17">
-        <v>1</v>
-      </c>
-      <c r="C44" s="16" t="s">
+      <c r="B44" s="13">
+        <v>1</v>
+      </c>
+      <c r="C44" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="12" t="s">
         <v>130</v>
       </c>
-      <c r="E44" s="16" t="s">
+      <c r="E44" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="18" t="s">
+      <c r="F44" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="19"/>
+      <c r="G44" s="21"/>
       <c r="H44" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="B45" s="17">
-        <v>1</v>
-      </c>
-      <c r="C45" s="16" t="s">
+      <c r="B45" s="13">
+        <v>1</v>
+      </c>
+      <c r="C45" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="D45" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E45" s="16" t="s">
+      <c r="E45" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="18" t="s">
+      <c r="F45" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="19"/>
+      <c r="G45" s="21"/>
       <c r="H45" s="8" t="s">
         <v>26</v>
       </c>
       <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B46" s="17">
-        <v>1</v>
-      </c>
-      <c r="C46" s="16" t="s">
+      <c r="B46" s="13">
+        <v>1</v>
+      </c>
+      <c r="C46" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="D46" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="E46" s="16" t="s">
+      <c r="E46" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="18" t="s">
+      <c r="F46" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="19"/>
+      <c r="G46" s="21"/>
       <c r="H46" s="8" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B47" s="17">
-        <v>1</v>
-      </c>
-      <c r="C47" s="16" t="s">
+      <c r="B47" s="13">
+        <v>1</v>
+      </c>
+      <c r="C47" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="12" t="s">
         <v>133</v>
       </c>
-      <c r="E47" s="16" t="s">
+      <c r="E47" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="18" t="s">
+      <c r="F47" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="19"/>
+      <c r="G47" s="21"/>
       <c r="H47" s="8" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="16" t="s">
+      <c r="A48" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="B48" s="17">
-        <v>1</v>
-      </c>
-      <c r="C48" s="16" t="s">
+      <c r="B48" s="13">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="18" t="s">
+      <c r="F48" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="19"/>
+      <c r="G48" s="21"/>
       <c r="H48" s="8" t="s">
         <v>26</v>
       </c>
@@ -1984,10 +1993,10 @@
       <c r="E49" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="10" t="s">
+      <c r="F49" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="11"/>
+      <c r="G49" s="17"/>
       <c r="H49" s="8" t="s">
         <v>55</v>
       </c>
@@ -2030,10 +2039,10 @@
       <c r="E51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="G51" s="11"/>
+      <c r="G51" s="17"/>
       <c r="H51" s="8" t="s">
         <v>26</v>
       </c>
@@ -2128,36 +2137,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F36:G36"/>
@@ -2167,10 +2146,41 @@
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
convert to JLC BOM format
</commit_message>
<xml_diff>
--- a/eps-eda/bom/eps_BOM.xlsx
+++ b/eps-eda/bom/eps_BOM.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igeorgi1\git-repos\coloradocube\eps\eps-eda\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EE5155-4E55-4383-BC59-E7060E28980E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C0FA8-386F-46A3-B9D5-F0C9CB875385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="180" windowWidth="24045" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="210" windowWidth="26310" windowHeight="13620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eps_masterBOM" sheetId="2" r:id="rId1"/>
+    <sheet name="eps_masterBOM (2)" sheetId="3" r:id="rId2"/>
+    <sheet name="JLC" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="208">
   <si>
     <t>FZT688BTA</t>
   </si>
@@ -528,12 +530,150 @@
   <si>
     <t>pic18f27:PIC18F27Q84-E&amp;slash_SP</t>
   </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>JLSPCB Part #</t>
+  </si>
+  <si>
+    <t>10uF, C_Small, Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>0.1uF, C_Small, Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>2.2uF, C_Small, Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>22uF, C, Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>0.1uF, C, Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>0.47uF, C_Small, Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>100nF, C, Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>4.7nF, C, Unpolarized capacitor</t>
+  </si>
+  <si>
+    <t>22uF, C2012X5R1A226M125AB, Unpolarized capacitor, small symbol</t>
+  </si>
+  <si>
+    <t>LED, LED, Light emitting diode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD3Z284C3V6-7, PD3Z284C3V6-7, </t>
+  </si>
+  <si>
+    <t>RED, LED_Small_Filled, Light emitting diode, small symbol, filled shape</t>
+  </si>
+  <si>
+    <t>GREEN, LED_Small_Filled, Light emitting diode, small symbol, filled shape</t>
+  </si>
+  <si>
+    <t>YELLOW, LED_Small_Filled, Light emitting diode, small symbol, filled shape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PD3S230LQ-7, PD3S230LQ-7, </t>
+  </si>
+  <si>
+    <t>DIODE, DIODE, Diode, anode on pin 1, for simulation only!</t>
+  </si>
+  <si>
+    <t>12401610E4#2A, USB_C_Receptacle, USB Full-Featured Type-C Receptacle connector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">436500212, 436500212, </t>
+  </si>
+  <si>
+    <t>826632-2, Conn_02x20_Odd_Even, Generic connector, double row, 02x20, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>PH1RB-05-UA, Conn_01x05_Female, Generic connector, single row, 01x05, script generated (kicad-library-utils/schlib/autogen/connector/)</t>
+  </si>
+  <si>
+    <t>SolderJumper_2_Open, SolderJumper_2_Open, Solder Jumper, 2-pole, open</t>
+  </si>
+  <si>
+    <t>.47uH, CIGT252010LMR47MNE, Inductor, small symbol</t>
+  </si>
+  <si>
+    <t xml:space="preserve">744316100, 744316100, </t>
+  </si>
+  <si>
+    <t>FZT688BTA, 2N2219, 800mA Ic, 50V Vce, NPN Transistor, TO-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSF4NTEBL500F, PSF4NTEBL500F, </t>
+  </si>
+  <si>
+    <t>10k, R_Small_US, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>1k, R_Small_US, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>24.9k, R_Small_US, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>0.01, R_Small_US, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>60, R, Resistor</t>
+  </si>
+  <si>
+    <t>10k, R, Resistor</t>
+  </si>
+  <si>
+    <t>200, R, Resistor</t>
+  </si>
+  <si>
+    <t>330, R, Resistor</t>
+  </si>
+  <si>
+    <t>732K, RMCF0603FG732K, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>100k, KTR03EZPF1003, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>453k, RMCF0603FT453K, Resistor, small US symbol</t>
+  </si>
+  <si>
+    <t>10k, NTCS0603E3103HLT, Temperature dependent resistor, negative temperature coefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS61022RWUR, TPS61022RWUR, </t>
+  </si>
+  <si>
+    <t>INA3221AIRGVR, INA3221, Triple-Channel High-Side Shunt and Bus Voltage Monitor with I2C and SMBUS Compatible Interface, QFN-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX77757JEFG435+, MAX77757JEFG435+, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX17055ETB+T, MAX17055ETB+T, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ATA6560-GAQW-VAO, ATA6560-GAQW-VAO, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIC18F27Q84-E/SP, PIC18F27Q84-E{slash}SP, </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -579,8 +719,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -605,6 +753,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -618,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -650,11 +804,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,8 +1043,8 @@
   </sheetPr>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
@@ -896,11 +1064,11 @@
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -909,10 +1077,10 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="17"/>
+      <c r="C2" s="23"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -922,10 +1090,10 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="23"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
@@ -935,12 +1103,12 @@
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -965,22 +1133,22 @@
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E6" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="23" t="s">
+      <c r="F6" s="21" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="2"/>
@@ -1002,10 +1170,10 @@
       <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="19"/>
+      <c r="G7" s="28"/>
       <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
@@ -1027,10 +1195,10 @@
       <c r="E8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="19"/>
+      <c r="G8" s="28"/>
       <c r="H8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1051,10 +1219,10 @@
       <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="19"/>
+      <c r="G9" s="28"/>
       <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
@@ -1075,10 +1243,10 @@
       <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="19"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
@@ -1099,10 +1267,10 @@
       <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="19"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="8" t="s">
         <v>26</v>
       </c>
@@ -1123,10 +1291,10 @@
       <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="18" t="s">
+      <c r="F12" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="19"/>
+      <c r="G12" s="28"/>
       <c r="H12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1147,10 +1315,10 @@
       <c r="E13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="18" t="s">
+      <c r="F13" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="28"/>
       <c r="H13" s="8" t="s">
         <v>26</v>
       </c>
@@ -1171,10 +1339,10 @@
       <c r="E14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="8" t="s">
         <v>26</v>
       </c>
@@ -1195,10 +1363,10 @@
       <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="19"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="8" t="s">
         <v>26</v>
       </c>
@@ -1219,10 +1387,10 @@
       <c r="E16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="19"/>
+      <c r="G16" s="28"/>
       <c r="H16" s="8" t="s">
         <v>26</v>
       </c>
@@ -1243,10 +1411,10 @@
       <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="18" t="s">
+      <c r="F17" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="19"/>
+      <c r="G17" s="28"/>
       <c r="H17" s="8" t="s">
         <v>26</v>
       </c>
@@ -1267,10 +1435,10 @@
       <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="17"/>
+      <c r="G18" s="23"/>
       <c r="H18" s="9"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1311,10 +1479,10 @@
       <c r="E20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="17"/>
+      <c r="G20" s="23"/>
       <c r="H20" s="9"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1333,10 +1501,10 @@
       <c r="E21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="F21" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="17"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="9"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1355,10 +1523,10 @@
       <c r="E22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F22" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="17"/>
+      <c r="G22" s="23"/>
       <c r="H22" s="9"/>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1399,10 +1567,10 @@
       <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="17"/>
+      <c r="G24" s="23"/>
       <c r="H24" s="4" t="s">
         <v>71</v>
       </c>
@@ -1423,10 +1591,10 @@
       <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="16" t="s">
+      <c r="F25" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="17"/>
+      <c r="G25" s="23"/>
       <c r="H25" s="8" t="s">
         <v>55</v>
       </c>
@@ -1469,10 +1637,10 @@
       <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="16" t="s">
+      <c r="F27" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="17"/>
+      <c r="G27" s="23"/>
       <c r="H27" s="8" t="s">
         <v>55</v>
       </c>
@@ -1493,10 +1661,10 @@
       <c r="E28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="17"/>
+      <c r="G28" s="23"/>
       <c r="H28" s="8" t="s">
         <v>55</v>
       </c>
@@ -1517,10 +1685,10 @@
       <c r="E29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="16" t="s">
+      <c r="F29" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="17"/>
+      <c r="G29" s="23"/>
       <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
@@ -1541,10 +1709,10 @@
       <c r="E30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="16" t="s">
+      <c r="F30" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="17"/>
+      <c r="G30" s="23"/>
       <c r="H30" s="8" t="s">
         <v>55</v>
       </c>
@@ -1587,10 +1755,10 @@
       <c r="E32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="17"/>
+      <c r="G32" s="23"/>
       <c r="H32" s="8" t="s">
         <v>104</v>
       </c>
@@ -1633,10 +1801,10 @@
       <c r="E34" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="21"/>
+      <c r="G34" s="25"/>
       <c r="H34" s="8" t="s">
         <v>26</v>
       </c>
@@ -1657,10 +1825,10 @@
       <c r="E35" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="21"/>
+      <c r="G35" s="25"/>
       <c r="H35" s="8" t="s">
         <v>26</v>
       </c>
@@ -1681,10 +1849,10 @@
       <c r="E36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F36" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="21"/>
+      <c r="G36" s="25"/>
       <c r="H36" s="8" t="s">
         <v>26</v>
       </c>
@@ -1705,10 +1873,10 @@
       <c r="E37" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="21"/>
+      <c r="G37" s="25"/>
       <c r="H37" s="8" t="s">
         <v>26</v>
       </c>
@@ -1729,10 +1897,10 @@
       <c r="E38" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="21"/>
+      <c r="G38" s="25"/>
       <c r="H38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
@@ -1847,10 +2015,10 @@
       <c r="E43" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="21"/>
+      <c r="G43" s="25"/>
       <c r="H43" s="8" t="s">
         <v>26</v>
       </c>
@@ -1872,10 +2040,10 @@
       <c r="E44" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="21"/>
+      <c r="G44" s="25"/>
       <c r="H44" s="8" t="s">
         <v>55</v>
       </c>
@@ -1896,10 +2064,10 @@
       <c r="E45" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="20" t="s">
+      <c r="F45" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="21"/>
+      <c r="G45" s="25"/>
       <c r="H45" s="8" t="s">
         <v>26</v>
       </c>
@@ -1921,10 +2089,10 @@
       <c r="E46" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="21"/>
+      <c r="G46" s="25"/>
       <c r="H46" s="8" t="s">
         <v>55</v>
       </c>
@@ -1945,10 +2113,10 @@
       <c r="E47" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="20" t="s">
+      <c r="F47" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="21"/>
+      <c r="G47" s="25"/>
       <c r="H47" s="8" t="s">
         <v>26</v>
       </c>
@@ -1969,10 +2137,10 @@
       <c r="E48" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="20" t="s">
+      <c r="F48" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="21"/>
+      <c r="G48" s="25"/>
       <c r="H48" s="8" t="s">
         <v>26</v>
       </c>
@@ -1993,10 +2161,10 @@
       <c r="E49" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="17"/>
+      <c r="G49" s="23"/>
       <c r="H49" s="8" t="s">
         <v>55</v>
       </c>
@@ -2039,10 +2207,10 @@
       <c r="E51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="G51" s="17"/>
+      <c r="G51" s="23"/>
       <c r="H51" s="8" t="s">
         <v>26</v>
       </c>
@@ -2137,6 +2305,36 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F36:G36"/>
@@ -2146,36 +2344,6 @@
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2183,4 +2351,2497 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55A993FB-25A0-4985-B453-00214A43969E}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:L55"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I6" sqref="I6:L55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26" style="17" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="52.28515625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" style="17" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" style="17" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="17" customWidth="1"/>
+    <col min="10" max="10" width="24.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="60.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="12.5703125" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="23"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+    </row>
+    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="6">
+        <v>80</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="7"/>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="J6" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11">
+        <v>6</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="28"/>
+      <c r="H7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="1" t="str">
+        <f>_xlfn.CONCAT(C7,", ",D7,", ",F7)</f>
+        <v>10uF, C_Small, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J7" s="17" t="str">
+        <f>A7</f>
+        <v>C1, C2, C8, C10, C11, C12,</v>
+      </c>
+      <c r="K7" s="17" t="str">
+        <f>E7</f>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="11">
+        <v>1</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="28"/>
+      <c r="H8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="1" t="str">
+        <f t="shared" ref="I8:I55" si="0">_xlfn.CONCAT(C8,", ",D8,", ",F8)</f>
+        <v>0.1uF, C_Small, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J8" s="17" t="str">
+        <f t="shared" ref="J8:J55" si="1">A8</f>
+        <v>C3,</v>
+      </c>
+      <c r="K8" s="17" t="str">
+        <f t="shared" ref="K8:K55" si="2">E8</f>
+        <v>Capacitor_SMD:C_0402_1005Metric</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="11">
+        <v>3</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="28"/>
+      <c r="H9" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>2.2uF, C_Small, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J9" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C5, C6, C7,</v>
+      </c>
+      <c r="K9" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="28"/>
+      <c r="H10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0.1uF, C_Small, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J10" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C9,</v>
+      </c>
+      <c r="K10" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0402_1005Metric</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="11">
+        <v>2</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="28"/>
+      <c r="H11" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>22uF, C, Unpolarized capacitor</v>
+      </c>
+      <c r="J11" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C13, C20,</v>
+      </c>
+      <c r="K11" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="11">
+        <v>4</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="28"/>
+      <c r="H12" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0.1uF, C, Unpolarized capacitor</v>
+      </c>
+      <c r="J12" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C14, C18, C19, C21,</v>
+      </c>
+      <c r="K12" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="28"/>
+      <c r="H13" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0.47uF, C_Small, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J13" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C15,</v>
+      </c>
+      <c r="K13" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="28"/>
+      <c r="H14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>100nF, C, Unpolarized capacitor</v>
+      </c>
+      <c r="J14" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C16,</v>
+      </c>
+      <c r="K14" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="28"/>
+      <c r="H15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>4.7nF, C, Unpolarized capacitor</v>
+      </c>
+      <c r="J15" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>C17,</v>
+      </c>
+      <c r="K15" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="11">
+        <v>3</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="28"/>
+      <c r="H16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>22uF, C2012X5R1A226M125AB, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J16" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Ca1, Ca2, Ca3,</v>
+      </c>
+      <c r="K16" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0805_2012Metric</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="11">
+        <v>3</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="28"/>
+      <c r="H17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>22uF, C2012X5R1A226M125AB, Unpolarized capacitor, small symbol</v>
+      </c>
+      <c r="J17" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Cb1, Cb2, Cb3,</v>
+      </c>
+      <c r="K17" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Capacitor_SMD:C_0805_2012Metric</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="6">
+        <v>2</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>LED, LED, Light emitting diode</v>
+      </c>
+      <c r="J18" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>D1, D2,</v>
+      </c>
+      <c r="K18" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>LED_SMD:LED_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
+      <c r="H19" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PD3Z284C3V6-7, PD3Z284C3V6-7, </v>
+      </c>
+      <c r="J19" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>D4,</v>
+      </c>
+      <c r="K19" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>zener_ovp:PD3Z284C3V6-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="6">
+        <v>1</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="23"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>RED, LED_Small_Filled, Light emitting diode, small symbol, filled shape</v>
+      </c>
+      <c r="J20" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>D5,</v>
+      </c>
+      <c r="K20" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>LED_SMD:LED_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="6">
+        <v>1</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21" s="23"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>GREEN, LED_Small_Filled, Light emitting diode, small symbol, filled shape</v>
+      </c>
+      <c r="J21" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>D6,</v>
+      </c>
+      <c r="K21" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>LED_SMD:LED_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="6">
+        <v>3</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="23"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>YELLOW, LED_Small_Filled, Light emitting diode, small symbol, filled shape</v>
+      </c>
+      <c r="J22" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>D7, D8, D9,</v>
+      </c>
+      <c r="K22" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>LED_SMD:LED_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="6">
+        <v>1</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="16"/>
+      <c r="G23" s="16"/>
+      <c r="H23" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PD3S230LQ-7, PD3S230LQ-7, </v>
+      </c>
+      <c r="J23" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>D_3.3,</v>
+      </c>
+      <c r="K23" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>footprints3:PD3S230LQ-7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="30">
+        <v>1</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" s="32"/>
+      <c r="H24" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>DIODE, DIODE, Diode, anode on pin 1, for simulation only!</v>
+      </c>
+      <c r="J24" s="34" t="str">
+        <f t="shared" si="1"/>
+        <v>Din1,</v>
+      </c>
+      <c r="K24" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>Diode_SMD:D_0805_2012Metric</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="6">
+        <v>1</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" s="23"/>
+      <c r="H25" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>12401610E4#2A, USB_C_Receptacle, USB Full-Featured Type-C Receptacle connector</v>
+      </c>
+      <c r="J25" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>J1,</v>
+      </c>
+      <c r="K25" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Connector_USB:USB_C_Receptacle_Amphenol_12401610E4-2A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B26" s="6">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6">
+        <v>436500212</v>
+      </c>
+      <c r="D26" s="6">
+        <v>436500212</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">436500212, 436500212, </v>
+      </c>
+      <c r="J26" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>J2,</v>
+      </c>
+      <c r="K26" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>molex connector:436500212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="E27" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" s="23"/>
+      <c r="H27" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>826632-2, Conn_02x20_Odd_Even, Generic connector, double row, 02x20, odd/even pin numbering scheme (row 1 odd numbers, row 2 even numbers), script generated (kicad-library-utils/schlib/autogen/connector/)</v>
+      </c>
+      <c r="J27" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>J3,</v>
+      </c>
+      <c r="K27" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Connector_PinHeader_2.54mm:PinHeader_2x20_P2.54mm_Vertical</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="6">
+        <v>1</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D28" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="E28" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>88</v>
+      </c>
+      <c r="G28" s="23"/>
+      <c r="H28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>PH1RB-05-UA, Conn_01x05_Female, Generic connector, single row, 01x05, script generated (kicad-library-utils/schlib/autogen/connector/)</v>
+      </c>
+      <c r="J28" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>J4,</v>
+      </c>
+      <c r="K28" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Connector_PinHeader_2.54mm:PinHeader_1x05_P2.54mm_Horizontal</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="B29" s="30">
+        <v>1</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="E29" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" s="32"/>
+      <c r="H29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I29" s="33" t="str">
+        <f t="shared" si="0"/>
+        <v>SolderJumper_2_Open, SolderJumper_2_Open, Solder Jumper, 2-pole, open</v>
+      </c>
+      <c r="J29" s="34" t="str">
+        <f t="shared" si="1"/>
+        <v>JP1,</v>
+      </c>
+      <c r="K29" s="34" t="str">
+        <f t="shared" si="2"/>
+        <v>Jumper:SolderJumper-2_P1.3mm_Bridged2Bar_Pad1.0x1.5mm</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="6">
+        <v>1</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="F30" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="23"/>
+      <c r="H30" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>.47uH, CIGT252010LMR47MNE, Inductor, small symbol</v>
+      </c>
+      <c r="J30" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>L1,</v>
+      </c>
+      <c r="K30" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Inductor_SMD:L_1008_2520Metric</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B31" s="6">
+        <v>2</v>
+      </c>
+      <c r="C31" s="6">
+        <v>744316100</v>
+      </c>
+      <c r="D31" s="6">
+        <v>744316100</v>
+      </c>
+      <c r="E31" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">744316100, 744316100, </v>
+      </c>
+      <c r="J31" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>L2, L3,</v>
+      </c>
+      <c r="K31" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>footprints1:744316100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="6">
+        <v>1</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="E32" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="23"/>
+      <c r="H32" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>FZT688BTA, 2N2219, 800mA Ic, 50V Vce, NPN Transistor, TO-39</v>
+      </c>
+      <c r="J32" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Q2,</v>
+      </c>
+      <c r="K32" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>fzt688bta_footprint:SOT230P700X180-4N</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B33" s="13">
+        <v>2</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PSF4NTEBL500F, PSF4NTEBL500F, </v>
+      </c>
+      <c r="J33" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R1, R2,</v>
+      </c>
+      <c r="K33" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>psf4nt:PSF4NTEBL500F</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B34" s="13">
+        <v>5</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G34" s="25"/>
+      <c r="H34" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10k, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J34" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R3, R4, R5, R6, R7,</v>
+      </c>
+      <c r="K34" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B35" s="13">
+        <v>2</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G35" s="25"/>
+      <c r="H35" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1k, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J35" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R8, R10,</v>
+      </c>
+      <c r="K35" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0402_1005Metric</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36" s="13">
+        <v>1</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G36" s="25"/>
+      <c r="H36" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>24.9k, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J36" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R9,</v>
+      </c>
+      <c r="K36" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0402_1005Metric</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="19" t="s">
+        <v>117</v>
+      </c>
+      <c r="B37" s="13">
+        <v>1</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G37" s="25"/>
+      <c r="H37" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10k, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J37" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R11,</v>
+      </c>
+      <c r="K37" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0402_1005Metric</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="B38" s="15">
+        <v>1</v>
+      </c>
+      <c r="C38" s="15">
+        <v>0.01</v>
+      </c>
+      <c r="D38" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G38" s="25"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>0.01, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J38" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R12,</v>
+      </c>
+      <c r="K38" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0805_2012Metric</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B39" s="13">
+        <v>2</v>
+      </c>
+      <c r="C39" s="13">
+        <v>60</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="19"/>
+      <c r="H39" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>60, R, Resistor</v>
+      </c>
+      <c r="J39" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R13, R14,</v>
+      </c>
+      <c r="K39" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="13">
+        <v>1</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G40" s="19"/>
+      <c r="H40" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10k, R, Resistor</v>
+      </c>
+      <c r="J40" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R15,</v>
+      </c>
+      <c r="K40" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="13">
+        <v>1</v>
+      </c>
+      <c r="C41" s="13">
+        <v>200</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G41" s="19"/>
+      <c r="H41" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>200, R, Resistor</v>
+      </c>
+      <c r="J41" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R16,</v>
+      </c>
+      <c r="K41" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B42" s="13">
+        <v>5</v>
+      </c>
+      <c r="C42" s="13">
+        <v>330</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" s="19"/>
+      <c r="H42" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>330, R, Resistor</v>
+      </c>
+      <c r="J42" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R19, R20, R21, R22, R23,</v>
+      </c>
+      <c r="K42" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B43" s="13">
+        <v>1</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F43" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G43" s="25"/>
+      <c r="H43" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>1k, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J43" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>R_3.3,</v>
+      </c>
+      <c r="K43" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B44" s="13">
+        <v>1</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F44" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="H44" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>732K, RMCF0603FG732K, Resistor, small US symbol</v>
+      </c>
+      <c r="J44" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Ra1,</v>
+      </c>
+      <c r="K44" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B45" s="13">
+        <v>1</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F45" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G45" s="25"/>
+      <c r="H45" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>100k, KTR03EZPF1003, Resistor, small US symbol</v>
+      </c>
+      <c r="J45" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Ra2,</v>
+      </c>
+      <c r="K45" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="13">
+        <v>1</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F46" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G46" s="25"/>
+      <c r="H46" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>453k, RMCF0603FT453K, Resistor, small US symbol</v>
+      </c>
+      <c r="J46" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Rb1,</v>
+      </c>
+      <c r="K46" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="13">
+        <v>1</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F47" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G47" s="25"/>
+      <c r="H47" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>100k, KTR03EZPF1003, Resistor, small US symbol</v>
+      </c>
+      <c r="J47" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Rb2,</v>
+      </c>
+      <c r="K47" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="B48" s="13">
+        <v>1</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F48" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="G48" s="25"/>
+      <c r="H48" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10k, R_Small_US, Resistor, small US symbol</v>
+      </c>
+      <c r="J48" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>Rpu1,</v>
+      </c>
+      <c r="K48" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B49" s="6">
+        <v>1</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="E49" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="F49" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="G49" s="23"/>
+      <c r="H49" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>10k, NTCS0603E3103HLT, Temperature dependent resistor, negative temperature coefficient</v>
+      </c>
+      <c r="J49" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>TH1,</v>
+      </c>
+      <c r="K49" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Resistor_SMD:R_0603_1608Metric</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="B50" s="6">
+        <v>2</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D50" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="F50" s="16"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">TPS61022RWUR, TPS61022RWUR, </v>
+      </c>
+      <c r="J50" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>U1, U2,</v>
+      </c>
+      <c r="K50" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>footprints:TPS61022RWUR</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="B51" s="6">
+        <v>1</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="F51" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="G51" s="23"/>
+      <c r="H51" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INA3221AIRGVR, INA3221, Triple-Channel High-Side Shunt and Bus Voltage Monitor with I2C and SMBUS Compatible Interface, QFN-16</v>
+      </c>
+      <c r="J51" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>U3,</v>
+      </c>
+      <c r="K51" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>Package_DFN_QFN:Texas_RGV_S-PVQFN-N16_EP2.1x2.1mm</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B52" s="6">
+        <v>1</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D52" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="F52" s="16"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">MAX77757JEFG435+, MAX77757JEFG435+, </v>
+      </c>
+      <c r="J52" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>U5,</v>
+      </c>
+      <c r="K52" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>max77757:IC_MAX77757JEFG435+</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B53" s="6">
+        <v>1</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="F53" s="16"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">MAX17055ETB+T, MAX17055ETB+T, </v>
+      </c>
+      <c r="J53" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>U6,</v>
+      </c>
+      <c r="K53" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>max17055 smd:MAX17055ETB&amp;plus_T</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="B54" s="6">
+        <v>1</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>157</v>
+      </c>
+      <c r="F54" s="16"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I54" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">ATA6560-GAQW-VAO, ATA6560-GAQW-VAO, </v>
+      </c>
+      <c r="J54" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>U7,</v>
+      </c>
+      <c r="K54" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>ata6560:ATA6560-GAQW-VAO</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B55" s="6">
+        <v>1</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="F55" s="16"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">PIC18F27Q84-E/SP, PIC18F27Q84-E{slash}SP, </v>
+      </c>
+      <c r="J55" s="17" t="str">
+        <f t="shared" si="1"/>
+        <v>U8,</v>
+      </c>
+      <c r="K55" s="17" t="str">
+        <f t="shared" si="2"/>
+        <v>pic18f27:PIC18F27Q84-E&amp;slash_SP</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="39">
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F8:G8"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1" xr:uid="{D22F4FAC-2965-4E91-A8A8-135A80C3C4BD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397FA090-883F-4A8C-9AB9-A06B152BCE2E}">
+  <dimension ref="A1:D50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="65.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="35" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>172</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>173</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>176</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>177</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>184</v>
+      </c>
+      <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+      <c r="C24" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>186</v>
+      </c>
+      <c r="B25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>187</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>188</v>
+      </c>
+      <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>189</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>191</v>
+      </c>
+      <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>192</v>
+      </c>
+      <c r="B31" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>193</v>
+      </c>
+      <c r="B33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C33" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>194</v>
+      </c>
+      <c r="B34" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>195</v>
+      </c>
+      <c r="B35" t="s">
+        <v>124</v>
+      </c>
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>197</v>
+      </c>
+      <c r="B37" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>191</v>
+      </c>
+      <c r="B38" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>198</v>
+      </c>
+      <c r="B39" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>199</v>
+      </c>
+      <c r="B40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>200</v>
+      </c>
+      <c r="B41" t="s">
+        <v>134</v>
+      </c>
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>199</v>
+      </c>
+      <c r="B42" t="s">
+        <v>137</v>
+      </c>
+      <c r="C42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>190</v>
+      </c>
+      <c r="B43" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>201</v>
+      </c>
+      <c r="B44" t="s">
+        <v>139</v>
+      </c>
+      <c r="C44" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>202</v>
+      </c>
+      <c r="B45" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" t="s">
+        <v>145</v>
+      </c>
+      <c r="C46" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>204</v>
+      </c>
+      <c r="B47" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>205</v>
+      </c>
+      <c r="B48" t="s">
+        <v>152</v>
+      </c>
+      <c r="C48" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>206</v>
+      </c>
+      <c r="B49" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" t="s">
+        <v>161</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
JLC part number or order source
</commit_message>
<xml_diff>
--- a/eps-eda/bom/eps_BOM.xlsx
+++ b/eps-eda/bom/eps_BOM.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\igeorgi1\git-repos\coloradocube\eps\eps-eda\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789C0FA8-386F-46A3-B9D5-F0C9CB875385}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA65B3B7-A61B-47AC-8D95-4ED3A18D7673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="210" windowWidth="26310" windowHeight="13620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-120" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="eps_masterBOM" sheetId="2" r:id="rId1"/>
     <sheet name="eps_masterBOM (2)" sheetId="3" r:id="rId2"/>
-    <sheet name="JLC" sheetId="4" r:id="rId3"/>
+    <sheet name="eps_BOM_JLCPCB" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="257">
   <si>
     <t>FZT688BTA</t>
   </si>
@@ -82,6 +82,7 @@
         <sz val="10"/>
         <color rgb="FF1155CC"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t>https://jlcpcb.com/parts/componentSearch</t>
     </r>
@@ -667,13 +668,160 @@
   </si>
   <si>
     <t xml:space="preserve">PIC18F27Q84-E/SP, PIC18F27Q84-E{slash}SP, </t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Remove?</t>
+  </si>
+  <si>
+    <t>Remove</t>
+  </si>
+  <si>
+    <t>C19702</t>
+  </si>
+  <si>
+    <t>C1525</t>
+  </si>
+  <si>
+    <t>C23630</t>
+  </si>
+  <si>
+    <t>C59461</t>
+  </si>
+  <si>
+    <t>C14663</t>
+  </si>
+  <si>
+    <t>C1623</t>
+  </si>
+  <si>
+    <t>C53987</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/diodes-incorporated/PD3Z284C3V6-7/1629585</t>
+  </si>
+  <si>
+    <t>DigiKey</t>
+  </si>
+  <si>
+    <t>C2286</t>
+  </si>
+  <si>
+    <t>C72043</t>
+  </si>
+  <si>
+    <t>C72038</t>
+  </si>
+  <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/PD3S230HQ-7?qs=gAfoL%252BRo%2FrJZ9ppNTG9EUw%3D%3D&amp;gclid=Cj0KCQjwg_iTBhDrARIsAD3Ib5jRgPMohVMwP67TjsqVI4CcMkA-9xdwyWxyxk9IlULmDBdqxeO0x_kaAljFEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/amphenol-commercial-products/12401610E4%232A/5775520?utm_adgroup=Connectors%20%26%20Interconnects&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Product&amp;utm_term=&amp;utm_content=Connectors%20%26%20Interconnects&amp;gclid=Cj0KCQjwg_iTBhDrARIsAD3Ib5jil7b4iTauOlmXcjh3GTmQdR8vnOEj5yy4wDzIgzFAf_WFe2sAasYaArcDEALw_wcB</t>
+  </si>
+  <si>
+    <t>C240839</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/te-connectivity-amp-connectors/826632-2/2276129</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adam-tech/PH1RB-06-UA/9830592?utm_adgroup=Rectangular%20Connectors%20-%20Headers%2C%20Male%20Pins&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Shopping_Product_Connectors%2C%20Interconnects_NEW&amp;utm_term=&amp;utm_content=Rectangular%20Connectors%20-%20Headers%2C%20Male%20Pins&amp;gclid=Cj0KCQjwg_iTBhDrARIsAD3Ib5hurzehwVgiZeuCTpjbt89EZIal5sK7iCq9wJV7_ChPMWEs17dTAvMaAijQEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samsung-electro-mechanics/CIGT252010LMR47MNE/7041266</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/TDK/C2012X5R1A226M125AB?qs=LcTL%2F5vFEzEl81ah%2FUQuuw%3D%3D&amp;gclid=Cj0KCQjwg_iTBhDrARIsAD3Ib5gaZA6YmsnRAvJyWV5w4hqqGU55CUnDo1qyXDQ_qc8bfcYhG7hDpj8aAjOrEALw_wcB</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Wurth-Elektronik/744316100?qs=%252B7BPNfeNhvUGKrgWBoCWwA%3D%3D</t>
+  </si>
+  <si>
+    <t>C460087</t>
+  </si>
+  <si>
+    <t>https://www.mouser.com/ProductDetail/Diodes-Incorporated/FZT688BTA?qs=Fd5IDHV0WqxCjVtHKYqUuw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/koa-speer-electronics-inc/PSF4NTEBL500F/12728476?utm_adgroup=Resistors&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Dynamic%20Search_EN_Product&amp;utm_term=&amp;utm_content=Resistors&amp;gclid=Cj0KCQjwg_iTBhDrARIsAD3Ib5gDnsEGqUFFhTZrJX0YqUOM2Ygz1lePSZCSiK-uMs-REvGeej4MXT0aAof5EALw_wcB</t>
+  </si>
+  <si>
+    <t>C25804</t>
+  </si>
+  <si>
+    <t>C11702</t>
+  </si>
+  <si>
+    <t>C25874</t>
+  </si>
+  <si>
+    <t>C25744</t>
+  </si>
+  <si>
+    <t>C8218</t>
+  </si>
+  <si>
+    <t>C23138</t>
+  </si>
+  <si>
+    <t>C728271</t>
+  </si>
+  <si>
+    <t>0.5W</t>
+  </si>
+  <si>
+    <t>C22764</t>
+  </si>
+  <si>
+    <t>C166918</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FG732K/1714225</t>
+  </si>
+  <si>
+    <t>C510119</t>
+  </si>
+  <si>
+    <t>C2484682</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stackpole-electronics-inc/RMCF0603FT453K/1761122?s=N4IgTCBcDaIEoFkDCAxADANjQZhQFQBYBWbAaRAF0BfIA</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/vishay-beyschlag-draloric-bc-components/NTCS0603E3103HLT/2615422?s=N4IgTCBcDaIHIBUDCBlADANjQZgKLYEYcAJAGQRAF0BfIA</t>
+  </si>
+  <si>
+    <t>C181255</t>
+  </si>
+  <si>
+    <t>OUT OF STOCK GLOBALLY</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc-maxim-integrated/MAX77757JEFG435/13978783</t>
+  </si>
+  <si>
+    <t>C402925</t>
+  </si>
+  <si>
+    <t>Surprisingly difficult to find</t>
+  </si>
+  <si>
+    <t>On hand</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -684,6 +832,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -691,25 +840,30 @@
       <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -726,6 +880,23 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="PingFangSC, PingFangSC-Semibold"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF999999"/>
+      <name val="PingFangSC, PingFangSC-Semibold"/>
     </font>
   </fonts>
   <fills count="6">
@@ -772,7 +943,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -807,22 +978,41 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1048,7 +1238,7 @@
       <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
@@ -1060,55 +1250,55 @@
     <col min="8" max="8" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="4" t="s">
@@ -1118,7 +1308,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
@@ -1132,7 +1322,7 @@
       <c r="G5" s="3"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
@@ -1154,7 +1344,7 @@
       <c r="G6" s="2"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>21</v>
       </c>
@@ -1170,16 +1360,16 @@
       <c r="E7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1195,15 +1385,15 @@
       <c r="E8" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>30</v>
       </c>
@@ -1219,15 +1409,15 @@
       <c r="E9" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1">
       <c r="A10" s="10" t="s">
         <v>32</v>
       </c>
@@ -1243,15 +1433,15 @@
       <c r="E10" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>34</v>
       </c>
@@ -1267,15 +1457,15 @@
       <c r="E11" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="28"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" customHeight="1">
       <c r="A12" s="10" t="s">
         <v>38</v>
       </c>
@@ -1291,15 +1481,15 @@
       <c r="E12" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="28"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" customHeight="1">
       <c r="A13" s="10" t="s">
         <v>39</v>
       </c>
@@ -1315,15 +1505,15 @@
       <c r="E13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="28"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" customHeight="1">
       <c r="A14" s="10" t="s">
         <v>41</v>
       </c>
@@ -1339,15 +1529,15 @@
       <c r="E14" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" customHeight="1">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
@@ -1363,15 +1553,15 @@
       <c r="E15" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="28"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" customHeight="1">
       <c r="A16" s="10" t="s">
         <v>45</v>
       </c>
@@ -1387,15 +1577,15 @@
       <c r="E16" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="28"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1">
       <c r="A17" s="10" t="s">
         <v>48</v>
       </c>
@@ -1411,15 +1601,15 @@
       <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="28"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1">
       <c r="A18" s="2" t="s">
         <v>49</v>
       </c>
@@ -1435,13 +1625,13 @@
       <c r="E18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="23"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>53</v>
       </c>
@@ -1463,7 +1653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>56</v>
       </c>
@@ -1479,13 +1669,13 @@
       <c r="E20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="23"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="9"/>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -1501,13 +1691,13 @@
       <c r="E21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="9"/>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>62</v>
       </c>
@@ -1523,13 +1713,13 @@
       <c r="E22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="23"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="9"/>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
         <v>64</v>
       </c>
@@ -1551,7 +1741,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
         <v>67</v>
       </c>
@@ -1567,15 +1757,15 @@
       <c r="E24" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="23"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1">
       <c r="A25" s="2" t="s">
         <v>72</v>
       </c>
@@ -1591,15 +1781,15 @@
       <c r="E25" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="23"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1">
       <c r="A26" s="2" t="s">
         <v>77</v>
       </c>
@@ -1621,7 +1811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
         <v>79</v>
       </c>
@@ -1637,15 +1827,15 @@
       <c r="E27" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="23"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1">
       <c r="A28" s="2" t="s">
         <v>84</v>
       </c>
@@ -1661,15 +1851,15 @@
       <c r="E28" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="23"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
         <v>89</v>
       </c>
@@ -1685,15 +1875,15 @@
       <c r="E29" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="23"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="A30" s="2" t="s">
         <v>93</v>
       </c>
@@ -1709,15 +1899,15 @@
       <c r="E30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="23"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
         <v>98</v>
       </c>
@@ -1739,7 +1929,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
         <v>100</v>
       </c>
@@ -1755,15 +1945,15 @@
       <c r="E32" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="23"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="8" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33" s="12" t="s">
         <v>105</v>
       </c>
@@ -1785,7 +1975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34" s="12" t="s">
         <v>107</v>
       </c>
@@ -1801,15 +1991,15 @@
       <c r="E34" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="32"/>
       <c r="H34" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35" s="12" t="s">
         <v>112</v>
       </c>
@@ -1825,15 +2015,15 @@
       <c r="E35" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="25"/>
+      <c r="G35" s="32"/>
       <c r="H35" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36" s="12" t="s">
         <v>115</v>
       </c>
@@ -1849,15 +2039,15 @@
       <c r="E36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="25"/>
+      <c r="G36" s="32"/>
       <c r="H36" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37" s="12" t="s">
         <v>117</v>
       </c>
@@ -1873,15 +2063,15 @@
       <c r="E37" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="25"/>
+      <c r="G37" s="32"/>
       <c r="H37" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38" s="14" t="s">
         <v>119</v>
       </c>
@@ -1897,13 +2087,13 @@
       <c r="E38" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="25"/>
+      <c r="G38" s="32"/>
       <c r="H38" s="9"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39" s="12" t="s">
         <v>121</v>
       </c>
@@ -1927,7 +2117,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40" s="12" t="s">
         <v>124</v>
       </c>
@@ -1951,7 +2141,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41" s="12" t="s">
         <v>125</v>
       </c>
@@ -1975,7 +2165,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42" s="12" t="s">
         <v>126</v>
       </c>
@@ -1999,7 +2189,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43" s="12" t="s">
         <v>127</v>
       </c>
@@ -2015,16 +2205,16 @@
       <c r="E43" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="25"/>
+      <c r="G43" s="32"/>
       <c r="H43" s="8" t="s">
         <v>26</v>
       </c>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44" s="12" t="s">
         <v>128</v>
       </c>
@@ -2040,15 +2230,15 @@
       <c r="E44" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="25"/>
+      <c r="G44" s="32"/>
       <c r="H44" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45" s="12" t="s">
         <v>131</v>
       </c>
@@ -2064,16 +2254,16 @@
       <c r="E45" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="25"/>
+      <c r="G45" s="32"/>
       <c r="H45" s="8" t="s">
         <v>26</v>
       </c>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46" s="12" t="s">
         <v>134</v>
       </c>
@@ -2089,15 +2279,15 @@
       <c r="E46" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F46" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="25"/>
+      <c r="G46" s="32"/>
       <c r="H46" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47" s="12" t="s">
         <v>137</v>
       </c>
@@ -2113,15 +2303,15 @@
       <c r="E47" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="25"/>
+      <c r="G47" s="32"/>
       <c r="H47" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48" s="12" t="s">
         <v>138</v>
       </c>
@@ -2137,15 +2327,15 @@
       <c r="E48" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="24" t="s">
+      <c r="F48" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="25"/>
+      <c r="G48" s="32"/>
       <c r="H48" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8">
       <c r="A49" s="2" t="s">
         <v>139</v>
       </c>
@@ -2161,15 +2351,15 @@
       <c r="E49" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F49" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="23"/>
+      <c r="G49" s="28"/>
       <c r="H49" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8">
       <c r="A50" s="2" t="s">
         <v>142</v>
       </c>
@@ -2191,7 +2381,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8">
       <c r="A51" s="2" t="s">
         <v>145</v>
       </c>
@@ -2207,15 +2397,15 @@
       <c r="E51" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="22" t="s">
+      <c r="F51" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="G51" s="23"/>
+      <c r="G51" s="28"/>
       <c r="H51" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8">
       <c r="A52" s="2" t="s">
         <v>149</v>
       </c>
@@ -2237,7 +2427,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8">
       <c r="A53" s="2" t="s">
         <v>152</v>
       </c>
@@ -2259,7 +2449,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8">
       <c r="A54" s="2" t="s">
         <v>155</v>
       </c>
@@ -2281,7 +2471,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8">
       <c r="A55" s="2" t="s">
         <v>158</v>
       </c>
@@ -2305,36 +2495,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F48:G48"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="F51:G51"/>
     <mergeCell ref="F36:G36"/>
@@ -2344,6 +2504,36 @@
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
@@ -2360,12 +2550,12 @@
   </sheetPr>
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6:L55"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="26" style="17" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="17" bestFit="1" customWidth="1"/>
@@ -2381,55 +2571,55 @@
     <col min="12" max="16384" width="12.5703125" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" customHeight="1">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="16"/>
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1">
       <c r="A2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="16"/>
       <c r="E2" s="16"/>
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15.75" customHeight="1">
       <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="23"/>
+      <c r="C3" s="28"/>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15.75" customHeight="1">
       <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="4" t="s">
@@ -2439,7 +2629,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="15.75" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
@@ -2453,7 +2643,7 @@
       <c r="G5" s="16"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="15.75" customHeight="1">
       <c r="A6" s="21" t="s">
         <v>15</v>
       </c>
@@ -2487,7 +2677,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>21</v>
       </c>
@@ -2503,10 +2693,10 @@
       <c r="E7" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="28"/>
+      <c r="G7" s="30"/>
       <c r="H7" s="9" t="s">
         <v>26</v>
       </c>
@@ -2523,7 +2713,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>27</v>
       </c>
@@ -2539,10 +2729,10 @@
       <c r="E8" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="28"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="9" t="s">
         <v>26</v>
       </c>
@@ -2559,7 +2749,7 @@
         <v>Capacitor_SMD:C_0402_1005Metric</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="15.75" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>30</v>
       </c>
@@ -2575,10 +2765,10 @@
       <c r="E9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="27" t="s">
+      <c r="F9" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="30"/>
       <c r="H9" s="9" t="s">
         <v>26</v>
       </c>
@@ -2595,7 +2785,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" ht="15.75" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>32</v>
       </c>
@@ -2611,10 +2801,10 @@
       <c r="E10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="27" t="s">
+      <c r="F10" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="28"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="9" t="s">
         <v>26</v>
       </c>
@@ -2631,7 +2821,7 @@
         <v>Capacitor_SMD:C_0402_1005Metric</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" ht="15.75" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>34</v>
       </c>
@@ -2647,10 +2837,10 @@
       <c r="E11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="27" t="s">
+      <c r="F11" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G11" s="28"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="9" t="s">
         <v>26</v>
       </c>
@@ -2667,7 +2857,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" ht="15.75" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>38</v>
       </c>
@@ -2683,10 +2873,10 @@
       <c r="E12" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="27" t="s">
+      <c r="F12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="28"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="9" t="s">
         <v>26</v>
       </c>
@@ -2703,7 +2893,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15.75" customHeight="1">
       <c r="A13" s="18" t="s">
         <v>39</v>
       </c>
@@ -2719,10 +2909,10 @@
       <c r="E13" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F13" s="27" t="s">
+      <c r="F13" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="28"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="9" t="s">
         <v>26</v>
       </c>
@@ -2739,7 +2929,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15.75" customHeight="1">
       <c r="A14" s="18" t="s">
         <v>41</v>
       </c>
@@ -2755,10 +2945,10 @@
       <c r="E14" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="28"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="9" t="s">
         <v>26</v>
       </c>
@@ -2775,7 +2965,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15.75" customHeight="1">
       <c r="A15" s="18" t="s">
         <v>43</v>
       </c>
@@ -2791,10 +2981,10 @@
       <c r="E15" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="27" t="s">
+      <c r="F15" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="28"/>
+      <c r="G15" s="30"/>
       <c r="H15" s="9" t="s">
         <v>26</v>
       </c>
@@ -2811,7 +3001,7 @@
         <v>Capacitor_SMD:C_0603_1608Metric</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15.75" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>45</v>
       </c>
@@ -2827,10 +3017,10 @@
       <c r="E16" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G16" s="28"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="9" t="s">
         <v>26</v>
       </c>
@@ -2847,7 +3037,7 @@
         <v>Capacitor_SMD:C_0805_2012Metric</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" customHeight="1">
       <c r="A17" s="18" t="s">
         <v>48</v>
       </c>
@@ -2863,10 +3053,10 @@
       <c r="E17" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="27" t="s">
+      <c r="F17" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="28"/>
+      <c r="G17" s="30"/>
       <c r="H17" s="9" t="s">
         <v>26</v>
       </c>
@@ -2883,7 +3073,7 @@
         <v>Capacitor_SMD:C_0805_2012Metric</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>49</v>
       </c>
@@ -2899,10 +3089,10 @@
       <c r="E18" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="23"/>
+      <c r="G18" s="28"/>
       <c r="H18" s="9"/>
       <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2917,7 +3107,7 @@
         <v>LED_SMD:LED_0603_1608Metric</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>53</v>
       </c>
@@ -2951,7 +3141,7 @@
         <v>zener_ovp:PD3Z284C3V6-7</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" customHeight="1">
       <c r="A20" s="16" t="s">
         <v>56</v>
       </c>
@@ -2967,10 +3157,10 @@
       <c r="E20" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G20" s="23"/>
+      <c r="G20" s="28"/>
       <c r="H20" s="9"/>
       <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2985,7 +3175,7 @@
         <v>LED_SMD:LED_0603_1608Metric</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" customHeight="1">
       <c r="A21" s="16" t="s">
         <v>60</v>
       </c>
@@ -3001,10 +3191,10 @@
       <c r="E21" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G21" s="23"/>
+      <c r="G21" s="28"/>
       <c r="H21" s="9"/>
       <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3019,7 +3209,7 @@
         <v>LED_SMD:LED_0603_1608Metric</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="16" t="s">
         <v>62</v>
       </c>
@@ -3035,10 +3225,10 @@
       <c r="E22" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="23"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="9"/>
       <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3053,7 +3243,7 @@
         <v>LED_SMD:LED_0603_1608Metric</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="16" t="s">
         <v>64</v>
       </c>
@@ -3087,43 +3277,43 @@
         <v>footprints3:PD3S230LQ-7</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="34" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+    <row r="24" spans="1:11" s="25" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A24" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B24" s="30">
-        <v>1</v>
-      </c>
-      <c r="C24" s="29" t="s">
+      <c r="B24" s="23">
+        <v>1</v>
+      </c>
+      <c r="C24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="G24" s="32"/>
+      <c r="G24" s="35"/>
       <c r="H24" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I24" s="33" t="str">
+      <c r="I24" s="24" t="str">
         <f t="shared" si="0"/>
         <v>DIODE, DIODE, Diode, anode on pin 1, for simulation only!</v>
       </c>
-      <c r="J24" s="34" t="str">
+      <c r="J24" s="25" t="str">
         <f t="shared" si="1"/>
         <v>Din1,</v>
       </c>
-      <c r="K24" s="34" t="str">
+      <c r="K24" s="25" t="str">
         <f t="shared" si="2"/>
         <v>Diode_SMD:D_0805_2012Metric</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="16" t="s">
         <v>72</v>
       </c>
@@ -3139,10 +3329,10 @@
       <c r="E25" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="G25" s="23"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="9" t="s">
         <v>55</v>
       </c>
@@ -3159,7 +3349,7 @@
         <v>Connector_USB:USB_C_Receptacle_Amphenol_12401610E4-2A</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="16" t="s">
         <v>77</v>
       </c>
@@ -3193,7 +3383,7 @@
         <v>molex connector:436500212</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" customHeight="1">
       <c r="A27" s="16" t="s">
         <v>79</v>
       </c>
@@ -3209,10 +3399,10 @@
       <c r="E27" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="G27" s="23"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="9" t="s">
         <v>55</v>
       </c>
@@ -3229,7 +3419,7 @@
         <v>Connector_PinHeader_2.54mm:PinHeader_2x20_P2.54mm_Vertical</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
       <c r="A28" s="16" t="s">
         <v>84</v>
       </c>
@@ -3245,10 +3435,10 @@
       <c r="E28" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="23"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="9" t="s">
         <v>55</v>
       </c>
@@ -3265,43 +3455,43 @@
         <v>Connector_PinHeader_2.54mm:PinHeader_1x05_P2.54mm_Horizontal</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+    <row r="29" spans="1:11" s="25" customFormat="1">
+      <c r="A29" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="B29" s="30">
-        <v>1</v>
-      </c>
-      <c r="C29" s="29" t="s">
+      <c r="B29" s="23">
+        <v>1</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="E29" s="29" t="s">
+      <c r="E29" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F29" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="G29" s="32"/>
+      <c r="G29" s="35"/>
       <c r="H29" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="I29" s="33" t="str">
+      <c r="I29" s="24" t="str">
         <f t="shared" si="0"/>
         <v>SolderJumper_2_Open, SolderJumper_2_Open, Solder Jumper, 2-pole, open</v>
       </c>
-      <c r="J29" s="34" t="str">
+      <c r="J29" s="25" t="str">
         <f t="shared" si="1"/>
         <v>JP1,</v>
       </c>
-      <c r="K29" s="34" t="str">
+      <c r="K29" s="25" t="str">
         <f t="shared" si="2"/>
         <v>Jumper:SolderJumper-2_P1.3mm_Bridged2Bar_Pad1.0x1.5mm</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11">
       <c r="A30" s="16" t="s">
         <v>93</v>
       </c>
@@ -3317,10 +3507,10 @@
       <c r="E30" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="G30" s="23"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="9" t="s">
         <v>55</v>
       </c>
@@ -3337,7 +3527,7 @@
         <v>Inductor_SMD:L_1008_2520Metric</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11">
       <c r="A31" s="16" t="s">
         <v>98</v>
       </c>
@@ -3371,7 +3561,7 @@
         <v>footprints1:744316100</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11">
       <c r="A32" s="16" t="s">
         <v>100</v>
       </c>
@@ -3387,10 +3577,10 @@
       <c r="E32" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="27" t="s">
         <v>103</v>
       </c>
-      <c r="G32" s="23"/>
+      <c r="G32" s="28"/>
       <c r="H32" s="9" t="s">
         <v>104</v>
       </c>
@@ -3407,7 +3597,7 @@
         <v>fzt688bta_footprint:SOT230P700X180-4N</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11">
       <c r="A33" s="19" t="s">
         <v>105</v>
       </c>
@@ -3441,7 +3631,7 @@
         <v>psf4nt:PSF4NTEBL500F</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11">
       <c r="A34" s="19" t="s">
         <v>107</v>
       </c>
@@ -3457,10 +3647,10 @@
       <c r="E34" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F34" s="24" t="s">
+      <c r="F34" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G34" s="25"/>
+      <c r="G34" s="32"/>
       <c r="H34" s="9" t="s">
         <v>26</v>
       </c>
@@ -3477,7 +3667,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11">
       <c r="A35" s="19" t="s">
         <v>112</v>
       </c>
@@ -3493,10 +3683,10 @@
       <c r="E35" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F35" s="24" t="s">
+      <c r="F35" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G35" s="25"/>
+      <c r="G35" s="32"/>
       <c r="H35" s="9" t="s">
         <v>26</v>
       </c>
@@ -3513,7 +3703,7 @@
         <v>Resistor_SMD:R_0402_1005Metric</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11">
       <c r="A36" s="19" t="s">
         <v>115</v>
       </c>
@@ -3529,10 +3719,10 @@
       <c r="E36" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F36" s="24" t="s">
+      <c r="F36" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G36" s="25"/>
+      <c r="G36" s="32"/>
       <c r="H36" s="9" t="s">
         <v>26</v>
       </c>
@@ -3549,7 +3739,7 @@
         <v>Resistor_SMD:R_0402_1005Metric</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11">
       <c r="A37" s="19" t="s">
         <v>117</v>
       </c>
@@ -3565,10 +3755,10 @@
       <c r="E37" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F37" s="24" t="s">
+      <c r="F37" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G37" s="25"/>
+      <c r="G37" s="32"/>
       <c r="H37" s="9" t="s">
         <v>26</v>
       </c>
@@ -3585,7 +3775,7 @@
         <v>Resistor_SMD:R_0402_1005Metric</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11">
       <c r="A38" s="20" t="s">
         <v>119</v>
       </c>
@@ -3601,10 +3791,10 @@
       <c r="E38" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="F38" s="26" t="s">
+      <c r="F38" s="33" t="s">
         <v>111</v>
       </c>
-      <c r="G38" s="25"/>
+      <c r="G38" s="32"/>
       <c r="H38" s="9"/>
       <c r="I38" s="1" t="str">
         <f t="shared" si="0"/>
@@ -3619,7 +3809,7 @@
         <v>Resistor_SMD:R_0805_2012Metric</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11">
       <c r="A39" s="19" t="s">
         <v>121</v>
       </c>
@@ -3655,7 +3845,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11">
       <c r="A40" s="19" t="s">
         <v>124</v>
       </c>
@@ -3691,7 +3881,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11">
       <c r="A41" s="19" t="s">
         <v>125</v>
       </c>
@@ -3727,7 +3917,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11">
       <c r="A42" s="19" t="s">
         <v>126</v>
       </c>
@@ -3763,7 +3953,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11">
       <c r="A43" s="19" t="s">
         <v>127</v>
       </c>
@@ -3779,10 +3969,10 @@
       <c r="E43" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F43" s="24" t="s">
+      <c r="F43" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G43" s="25"/>
+      <c r="G43" s="32"/>
       <c r="H43" s="9" t="s">
         <v>26</v>
       </c>
@@ -3799,7 +3989,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11">
       <c r="A44" s="19" t="s">
         <v>128</v>
       </c>
@@ -3815,10 +4005,10 @@
       <c r="E44" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F44" s="24" t="s">
+      <c r="F44" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G44" s="25"/>
+      <c r="G44" s="32"/>
       <c r="H44" s="9" t="s">
         <v>55</v>
       </c>
@@ -3835,7 +4025,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11">
       <c r="A45" s="19" t="s">
         <v>131</v>
       </c>
@@ -3851,10 +4041,10 @@
       <c r="E45" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F45" s="24" t="s">
+      <c r="F45" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G45" s="25"/>
+      <c r="G45" s="32"/>
       <c r="H45" s="9" t="s">
         <v>26</v>
       </c>
@@ -3871,7 +4061,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11">
       <c r="A46" s="19" t="s">
         <v>134</v>
       </c>
@@ -3887,10 +4077,10 @@
       <c r="E46" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F46" s="24" t="s">
+      <c r="F46" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G46" s="25"/>
+      <c r="G46" s="32"/>
       <c r="H46" s="9" t="s">
         <v>55</v>
       </c>
@@ -3907,7 +4097,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11">
       <c r="A47" s="19" t="s">
         <v>137</v>
       </c>
@@ -3923,10 +4113,10 @@
       <c r="E47" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F47" s="24" t="s">
+      <c r="F47" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G47" s="25"/>
+      <c r="G47" s="32"/>
       <c r="H47" s="9" t="s">
         <v>26</v>
       </c>
@@ -3943,7 +4133,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11">
       <c r="A48" s="19" t="s">
         <v>138</v>
       </c>
@@ -3959,10 +4149,10 @@
       <c r="E48" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="F48" s="24" t="s">
+      <c r="F48" s="31" t="s">
         <v>111</v>
       </c>
-      <c r="G48" s="25"/>
+      <c r="G48" s="32"/>
       <c r="H48" s="9" t="s">
         <v>26</v>
       </c>
@@ -3979,7 +4169,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11">
       <c r="A49" s="16" t="s">
         <v>139</v>
       </c>
@@ -3995,10 +4185,10 @@
       <c r="E49" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F49" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="G49" s="23"/>
+      <c r="G49" s="28"/>
       <c r="H49" s="9" t="s">
         <v>55</v>
       </c>
@@ -4015,7 +4205,7 @@
         <v>Resistor_SMD:R_0603_1608Metric</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11">
       <c r="A50" s="16" t="s">
         <v>142</v>
       </c>
@@ -4049,7 +4239,7 @@
         <v>footprints:TPS61022RWUR</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11">
       <c r="A51" s="16" t="s">
         <v>145</v>
       </c>
@@ -4065,10 +4255,10 @@
       <c r="E51" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="F51" s="22" t="s">
+      <c r="F51" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="G51" s="23"/>
+      <c r="G51" s="28"/>
       <c r="H51" s="9" t="s">
         <v>26</v>
       </c>
@@ -4085,7 +4275,7 @@
         <v>Package_DFN_QFN:Texas_RGV_S-PVQFN-N16_EP2.1x2.1mm</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11">
       <c r="A52" s="16" t="s">
         <v>149</v>
       </c>
@@ -4119,7 +4309,7 @@
         <v>max77757:IC_MAX77757JEFG435+</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11">
       <c r="A53" s="16" t="s">
         <v>152</v>
       </c>
@@ -4153,7 +4343,7 @@
         <v>max17055 smd:MAX17055ETB&amp;plus_T</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11">
       <c r="A54" s="16" t="s">
         <v>155</v>
       </c>
@@ -4187,7 +4377,7 @@
         <v>ata6560:ATA6560-GAQW-VAO</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11">
       <c r="A55" s="16" t="s">
         <v>158</v>
       </c>
@@ -4223,6 +4413,36 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F36:G36"/>
     <mergeCell ref="F48:G48"/>
     <mergeCell ref="F49:G49"/>
     <mergeCell ref="F51:G51"/>
@@ -4232,36 +4452,6 @@
     <mergeCell ref="F45:G45"/>
     <mergeCell ref="F46:G46"/>
     <mergeCell ref="F47:G47"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F8:G8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="I4" r:id="rId1" xr:uid="{D22F4FAC-2965-4E91-A8A8-135A80C3C4BD}"/>
@@ -4273,571 +4463,872 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397FA090-883F-4A8C-9AB9-A06B152BCE2E}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="65.5703125" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.5703125" customWidth="1"/>
+    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="32" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="26" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="E1" s="26" t="s">
+        <v>208</v>
+      </c>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" ht="63.75">
+      <c r="A2" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2" s="38" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" spans="1:7" ht="14.25">
+      <c r="A3" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D3" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E3" s="36"/>
+    </row>
+    <row r="4" spans="1:7" ht="25.5">
+      <c r="A4" s="36" t="s">
         <v>167</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D4" s="38" t="s">
+        <v>213</v>
+      </c>
+      <c r="E4" s="36"/>
+    </row>
+    <row r="5" spans="1:7" ht="14.25">
+      <c r="A5" s="36" t="s">
         <v>166</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="D5" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="36"/>
+    </row>
+    <row r="6" spans="1:7" ht="25.5">
+      <c r="A6" s="36" t="s">
         <v>168</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="D6" s="38" t="s">
+        <v>214</v>
+      </c>
+      <c r="E6" s="36"/>
+    </row>
+    <row r="7" spans="1:7" ht="51">
+      <c r="A7" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="D7" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="E7" s="36"/>
+    </row>
+    <row r="8" spans="1:7" ht="14.25">
+      <c r="A8" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="D8" s="38" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="36"/>
+    </row>
+    <row r="9" spans="1:7" ht="14.25">
+      <c r="A9" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="D9" s="38" t="s">
+        <v>215</v>
+      </c>
+      <c r="E9" s="36"/>
+    </row>
+    <row r="10" spans="1:7" ht="14.25">
+      <c r="A10" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="D10" s="38" t="s">
+        <v>217</v>
+      </c>
+      <c r="E10" s="36"/>
+    </row>
+    <row r="11" spans="1:7" ht="38.25">
+      <c r="A11" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="36" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="D11" s="38"/>
+      <c r="E11" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="F11" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G11" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="38.25">
+      <c r="A12" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="36" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="D12" s="38"/>
+      <c r="E12" s="38" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.25">
+      <c r="A13" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="D13" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" ht="14.25">
+      <c r="A14" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="36" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D14" s="39"/>
+      <c r="E14" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G14" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25.5">
+      <c r="A15" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D15" s="38" t="s">
+        <v>221</v>
+      </c>
+      <c r="E15" s="36"/>
+    </row>
+    <row r="16" spans="1:7" ht="25.5">
+      <c r="A16" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="D16" s="38" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="36"/>
+    </row>
+    <row r="17" spans="1:7" ht="25.5">
+      <c r="A17" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="36" t="s">
         <v>62</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="36" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="D17" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="E17" s="36"/>
+    </row>
+    <row r="18" spans="1:7" ht="14.25">
+      <c r="A18" s="37" t="s">
         <v>179</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="36" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="D18" s="39"/>
+      <c r="E18" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="G18" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="25.5">
+      <c r="A19" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="36" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="D19" s="36"/>
+      <c r="E19" s="37" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="25.5">
+      <c r="A20" s="37" t="s">
         <v>181</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="36" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="D20" s="36"/>
+      <c r="E20" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14.25">
+      <c r="A21" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="36" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="D21" s="38" t="s">
+        <v>227</v>
+      </c>
+      <c r="E21" s="36"/>
+    </row>
+    <row r="22" spans="1:7" ht="51">
+      <c r="A22" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="36" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="D22" s="39"/>
+      <c r="E22" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F22" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G22" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="38.25">
+      <c r="A23" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="36" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="D23" s="36"/>
+      <c r="E23" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F23" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G23" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="38.25">
+      <c r="A24" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="36" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="D24" s="36"/>
+      <c r="E24" s="37" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="36" t="s">
         <v>93</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="36" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="D25" s="36"/>
+      <c r="E25" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F25" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G25" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="36" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="D26" s="36"/>
+      <c r="E26" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F26" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="25.5">
+      <c r="A27" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="36" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="D27" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F27" s="36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G27" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="14.25">
+      <c r="A28" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="36" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="D28" s="39"/>
+      <c r="E28" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F28" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G28" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="38.25">
+      <c r="A29" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="D29" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E29" s="36"/>
+    </row>
+    <row r="30" spans="1:7" ht="25.5">
+      <c r="A30" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="D30" s="38" t="s">
+        <v>237</v>
+      </c>
+      <c r="E30" s="36"/>
+    </row>
+    <row r="31" spans="1:7" ht="14.25">
+      <c r="A31" s="36" t="s">
         <v>192</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="D31" s="38" t="s">
+        <v>238</v>
+      </c>
+      <c r="E31" s="36"/>
+    </row>
+    <row r="32" spans="1:7" ht="14.25">
+      <c r="A32" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="36" t="s">
         <v>117</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="36" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D32" s="38" t="s">
+        <v>239</v>
+      </c>
+      <c r="E32" s="36"/>
+    </row>
+    <row r="33" spans="1:7" ht="14.25">
+      <c r="A33" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="36" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="D33" s="38" t="s">
+        <v>242</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="25" customFormat="1" ht="25.5">
+      <c r="A34" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="40" t="s">
         <v>121</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="40" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="D34" s="41" t="s">
+        <v>245</v>
+      </c>
+      <c r="E34" s="42" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="14.25">
+      <c r="A35" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="D35" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E35" s="36"/>
+    </row>
+    <row r="36" spans="1:7" ht="14.25">
+      <c r="A36" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="D36" s="38" t="s">
+        <v>240</v>
+      </c>
+      <c r="E36" s="36"/>
+    </row>
+    <row r="37" spans="1:7" ht="63.75">
+      <c r="A37" s="36" t="s">
         <v>197</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="36" t="s">
         <v>126</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+      <c r="D37" s="38" t="s">
+        <v>241</v>
+      </c>
+      <c r="E37" s="36"/>
+    </row>
+    <row r="38" spans="1:7" ht="14.25">
+      <c r="A38" s="36" t="s">
         <v>191</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="36" t="s">
         <v>127</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+      <c r="D38" s="38" t="s">
+        <v>244</v>
+      </c>
+      <c r="E38" s="36"/>
+    </row>
+    <row r="39" spans="1:7" ht="14.25">
+      <c r="A39" s="36" t="s">
         <v>198</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+      <c r="D39" s="39"/>
+      <c r="E39" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F39" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G39" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="14.25">
+      <c r="A40" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
+      <c r="D40" s="38" t="s">
+        <v>247</v>
+      </c>
+      <c r="E40" s="36"/>
+    </row>
+    <row r="41" spans="1:7" ht="14.25">
+      <c r="A41" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+      <c r="D41" s="38" t="s">
+        <v>248</v>
+      </c>
+      <c r="E41" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F41" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G41" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
+      <c r="A42" s="37" t="s">
         <v>199</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="D42" t="s">
+        <v>247</v>
+      </c>
+      <c r="F42" s="37"/>
+    </row>
+    <row r="43" spans="1:7" ht="14.25">
+      <c r="A43" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="D43" s="38" t="s">
+        <v>236</v>
+      </c>
+      <c r="E43" s="36"/>
+    </row>
+    <row r="44" spans="1:7" ht="25.5">
+      <c r="A44" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="36" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+      <c r="D44" s="39"/>
+      <c r="E44" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="F44" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="G44" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" s="25" customFormat="1" ht="25.5">
+      <c r="A45" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="40" t="s">
         <v>142</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="40" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
+      <c r="D45" s="40"/>
+      <c r="E45" s="40" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="38.25">
+      <c r="A46" s="37" t="s">
         <v>203</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="36" t="s">
         <v>145</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="36" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
+      <c r="D46" s="38" t="s">
+        <v>251</v>
+      </c>
+      <c r="E46" s="36"/>
+    </row>
+    <row r="47" spans="1:7" ht="14.25">
+      <c r="A47" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="36" t="s">
         <v>149</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="36" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
+      <c r="D47" s="39"/>
+      <c r="E47" s="36" t="s">
+        <v>218</v>
+      </c>
+      <c r="F47" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="G47" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" s="25" customFormat="1" ht="25.5">
+      <c r="A48" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="40" t="s">
         <v>152</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="40" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+      <c r="D48" s="41" t="s">
+        <v>254</v>
+      </c>
+      <c r="E48" s="42" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="14.25">
+      <c r="A49" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="36" t="s">
         <v>155</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="36" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="D49" s="39"/>
+      <c r="E49" s="37" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="36" t="s">
         <v>207</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="36" t="s">
         <v>161</v>
+      </c>
+      <c r="D50" s="36"/>
+      <c r="E50" s="37" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>